<commit_message>
Fix item order (submit preceded which)
</commit_message>
<xml_diff>
--- a/inst/formr/bvq-1.0.1/bvq_01_log.xlsx
+++ b/inst/formr/bvq-1.0.1/bvq_01_log.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggarciad\OneDrive - San Juan de Dios\Documentos\projects\bvq\inst\formr\bvq-1.0.1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,162 +28,142 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">block_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mc  many_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">language</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>showif</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>block_order</t>
+  </si>
+  <si>
+    <t>item_order</t>
+  </si>
+  <si>
+    <t>mc  many_choices</t>
+  </si>
+  <si>
+    <t>language</t>
   </si>
   <si>
     <t xml:space="preserve">get bl_code </t>
   </si>
   <si>
-    <t xml:space="preserve">bl_code</t>
+    <t>bl_code</t>
   </si>
   <si>
     <t xml:space="preserve">get version </t>
   </si>
   <si>
-    <t xml:space="preserve">version</t>
+    <t>version</t>
   </si>
   <si>
     <t xml:space="preserve">get which </t>
   </si>
   <si>
-    <t xml:space="preserve">which</t>
+    <t>which</t>
   </si>
   <si>
     <t xml:space="preserve">submit  </t>
   </si>
   <si>
-    <t xml:space="preserve">submit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Següent/Siguiente/Next</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">many_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Català</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spanish</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Español</t>
-  </si>
-  <si>
-    <t xml:space="preserve">english</t>
-  </si>
-  <si>
-    <t xml:space="preserve">English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maximum_number_displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">displayed_percentage_maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_percentage_points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enable_instant_validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expire_after</t>
-  </si>
-  <si>
-    <t xml:space="preserve">google_file_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unlinked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expire_invitation_after</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expire_invitation_grace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide_results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use_paging</t>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>Següent/Siguiente/Next</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>many_choices</t>
+  </si>
+  <si>
+    <t>catalan</t>
+  </si>
+  <si>
+    <t>Català</t>
+  </si>
+  <si>
+    <t>spanish</t>
+  </si>
+  <si>
+    <t>Español</t>
+  </si>
+  <si>
+    <t>english</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>maximum_number_displayed</t>
+  </si>
+  <si>
+    <t>displayed_percentage_maximum</t>
+  </si>
+  <si>
+    <t>add_percentage_points</t>
+  </si>
+  <si>
+    <t>enable_instant_validation</t>
+  </si>
+  <si>
+    <t>expire_after</t>
+  </si>
+  <si>
+    <t>google_file_id</t>
+  </si>
+  <si>
+    <t>unlinked</t>
+  </si>
+  <si>
+    <t>expire_invitation_after</t>
+  </si>
+  <si>
+    <t>expire_invitation_grace</t>
+  </si>
+  <si>
+    <t>hide_results</t>
+  </si>
+  <si>
+    <t>use_paging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -192,7 +176,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -200,96 +184,71 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -297,12 +256,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -331,7 +290,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -352,7 +311,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -403,7 +362,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -421,33 +380,32 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.25" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3"/>
+    <col min="1" max="2" width="20" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -472,52 +430,55 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="20" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -527,39 +488,29 @@
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>4</v>
+      <c r="I6">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30"/>
+    <col min="1" max="2" width="20" style="1"/>
+    <col min="3" max="3" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>20</v>
       </c>
@@ -570,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -581,7 +532,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -592,7 +543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -604,33 +555,23 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20"/>
+    <col min="1" max="2" width="20" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -639,89 +580,84 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>